<commit_message>
cambios readme item c
</commit_message>
<xml_diff>
--- a/ItemB/experimentacion.xlsx
+++ b/ItemB/experimentacion.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yared\Documents\proyectos\proyecto-paralela\proyecto-paralela\ItemB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016B2EF9-EF7B-4AE8-A553-5CC1794E3E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A5582C-A763-4D80-BDC0-A6C7F9AE8E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3312" yWindow="1644" windowWidth="17280" windowHeight="8880" xr2:uid="{67894863-655E-42DD-8B27-801B00FCFA2B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="tiempo de ejecución" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,9 +56,6 @@
     <t>n=16k</t>
   </si>
   <si>
-    <t>Tiempo en segundos</t>
-  </si>
-  <si>
     <t>n=8k (8192)</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>n=16k (16384)</t>
   </si>
   <si>
-    <t>(para 16k demoró para p=1 unos 5 minutos, debo bajar la escala. Puedo usar n=16k pero como el n más grande).</t>
-  </si>
-  <si>
     <t>n=9k</t>
   </si>
   <si>
@@ -114,6 +108,12 @@
   </si>
   <si>
     <t>n=15k</t>
+  </si>
+  <si>
+    <t>(se utilizó n=16k como máxim n porque demoraba más de 8 minutos para 1 proceso)</t>
+  </si>
+  <si>
+    <t>Tiempo de ejecución en segundos</t>
   </si>
 </sst>
 </file>
@@ -143,12 +143,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -158,7 +173,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45A83B8-72DC-4B37-8695-67A9EF4E6B24}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,7 +521,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -535,31 +550,31 @@
         <v>2</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="T2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -673,7 +688,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
         <v>40</v>
@@ -726,7 +741,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>36.234999999999999</v>
@@ -746,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <v>31.085000000000001</v>
@@ -789,7 +804,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>26.696000000000002</v>
@@ -810,31 +825,31 @@
         <v>2</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="T9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -842,7 +857,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>25.443999999999999</v>
@@ -895,7 +910,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>23.006</v>
@@ -948,7 +963,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>24.260999999999999</v>
@@ -1001,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1">
         <v>22.995999999999999</v>
@@ -1017,190 +1032,274 @@
       <c r="L13" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" t="s">
-        <v>8</v>
-      </c>
-      <c r="J20" t="s">
-        <v>9</v>
-      </c>
-      <c r="K20" t="s">
-        <v>10</v>
-      </c>
-      <c r="L20" t="s">
-        <v>11</v>
-      </c>
-      <c r="M20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <f>AVERAGE(C2:E2)</f>
         <v>107.14999999999999</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <f>AVERAGE(C3:E3)</f>
         <v>62.959000000000003</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <f>AVERAGE(C4:E4)</f>
         <v>41.209666666666664</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <f>AVERAGE(C5:E5)</f>
         <v>39.528333333333336</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <f>AVERAGE(C6:E6)</f>
         <v>35.449999999999996</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <f>AVERAGE(C7:E7)</f>
         <v>31.692666666666668</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="2">
         <f>AVERAGE(C8:E8)</f>
         <v>29.455000000000002</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="2">
         <f>AVERAGE(C9:E9)</f>
         <v>27.082999999999998</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="2">
         <f>AVERAGE(C10:E10)</f>
         <v>26.610666666666663</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="2">
         <f>AVERAGE(C11:E11)</f>
         <v>23.740666666666669</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="2">
         <f>AVERAGE(C12:E12)</f>
         <v>22.996666666666666</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="2">
         <f>AVERAGE(C13:E13)</f>
         <v>23.372666666666664</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2">
         <f>AVERAGE(I3:I5)</f>
         <v>140.77666666666667</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <f t="shared" ref="C22:M22" si="0">AVERAGE(J3:J5)</f>
         <v>74.459333333333333</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>48.198666666666668</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <f t="shared" si="0"/>
         <v>45.026666666666664</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <f t="shared" si="0"/>
         <v>42.006666666666661</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <f t="shared" si="0"/>
         <v>39.378999999999998</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="2">
         <f t="shared" si="0"/>
         <v>36.199333333333335</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="2">
         <f t="shared" si="0"/>
         <v>34.918333333333329</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="2">
         <f t="shared" si="0"/>
         <v>32.076999999999998</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="2">
         <f t="shared" si="0"/>
         <v>29.923666666666666</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="2">
         <f t="shared" si="0"/>
         <v>27.687333333333338</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="2">
         <f t="shared" si="0"/>
         <v>27.617999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>16</v>
+      <c r="A29" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B29" s="2">
         <f>AVERAGE(I10:I12)</f>
@@ -1254,5 +1353,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>